<commit_message>
Updates to Thunder Tests found from testing.  Updates to Spreadsheet
</commit_message>
<xml_diff>
--- a/thunder-tests/VSAC FHIR API Test Scenarios - Connectathon32-js.xlsx
+++ b/thunder-tests/VSAC FHIR API Test Scenarios - Connectathon32-js.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuareynolds/Documents/src/cqf-measures/thunder-tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31A9295E-45D9-8A4A-B778-C4C6E31E0B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D12020-10E5-C446-9729-E8330606372D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2271,8 +2271,8 @@
   <dimension ref="A1:K235"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C200" sqref="C200"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C210" sqref="C210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>